<commit_message>
fixing the input vars file
</commit_message>
<xml_diff>
--- a/lib/inputVars.xlsx
+++ b/lib/inputVars.xlsx
@@ -248,7 +248,7 @@
     <t>Only if (and, or)</t>
   </si>
   <si>
-    <t>Col 0</t>
+    <t>col 0</t>
   </si>
   <si>
     <t>none</t>
@@ -257,7 +257,7 @@
     <t>variable crossPercent 3</t>
   </si>
   <si>
-    <t>Col 1</t>
+    <t>col 1</t>
   </si>
   <si>
     <t>or</t>
@@ -272,13 +272,13 @@
     <t>crossAbove 10 200</t>
   </si>
   <si>
-    <t>Col 2</t>
+    <t>col 2</t>
   </si>
   <si>
     <t>topLine 10</t>
   </si>
   <si>
-    <t>Col 3</t>
+    <t>col 3</t>
   </si>
   <si>
     <t>and</t>
@@ -290,13 +290,13 @@
     <t>priceAbove 10 200</t>
   </si>
   <si>
-    <t>Col 4</t>
+    <t>col 4</t>
   </si>
   <si>
     <t>priceAbove 50 30</t>
   </si>
   <si>
-    <t>Col 5</t>
+    <t>col 5</t>
   </si>
   <si>
     <t>variable crossPercent 5</t>
@@ -305,16 +305,16 @@
     <t>crossAbove 10 30</t>
   </si>
   <si>
-    <t>Col 6</t>
-  </si>
-  <si>
-    <t>Col 7</t>
-  </si>
-  <si>
-    <t>Col 8</t>
-  </si>
-  <si>
-    <t>Col 9</t>
+    <t>col 6</t>
+  </si>
+  <si>
+    <t>col 7</t>
+  </si>
+  <si>
+    <t>col 8</t>
+  </si>
+  <si>
+    <t>col 9</t>
   </si>
   <si>
     <t>Section 3 input test</t>
@@ -568,8 +568,8 @@
   </sheetPr>
   <dimension ref="A4:X60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O46" activeCellId="0" sqref="O46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
works for both folers and files because of importer function cross var price has a below and above clause
</commit_message>
<xml_diff>
--- a/lib/inputVars.xlsx
+++ b/lib/inputVars.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="98">
   <si>
     <t>Signal Name</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Price</t>
   </si>
   <si>
+    <t>(above, below, both)</t>
+  </si>
+  <si>
     <t>CI</t>
   </si>
   <si>
@@ -36,6 +39,9 @@
   </si>
   <si>
     <t>+ or - </t>
+  </si>
+  <si>
+    <t>above</t>
   </si>
   <si>
     <t>&lt;&lt; number dollar price</t>
@@ -568,8 +574,8 @@
   </sheetPr>
   <dimension ref="A4:X60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,124 +604,130 @@
       <c r="F4" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="n">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="3" t="n">
         <v>0.01</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="3" t="n">
         <v>0.02</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="3" t="n">
         <v>0.03</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="3" t="n">
         <v>0.05</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="3" t="n">
         <v>0.03</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>3</v>
@@ -724,18 +736,18 @@
         <v>0.025</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>3</v>
@@ -744,18 +756,18 @@
         <v>0.025</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>3</v>
@@ -764,18 +776,18 @@
         <v>0.025</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>3</v>
@@ -784,53 +796,53 @@
         <v>0.025</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>0.02</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="3" t="n">
         <v>0.02</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>10</v>
@@ -839,162 +851,162 @@
         <v>0.05</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E21" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1003,7 +1015,7 @@
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>1</v>
@@ -1038,43 +1050,43 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
@@ -1088,159 +1100,159 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O44" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="O46" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O53" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>15</v>

</xml_diff>